<commit_message>
under repair: [Kinematics class ] DK not working properly.
</commit_message>
<xml_diff>
--- a/Actor_RobotObj_01.xlsx
+++ b/Actor_RobotObj_01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\waltz\Documents\CppProjects\GitManagements\QuantumCoreRobotRenew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{074F3146-73E5-4267-947B-6DCED1D5B501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{6736FA47-5E9A-4F07-8CDF-D36A6B0B9547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22395" yWindow="7860" windowWidth="18075" windowHeight="11040" xr2:uid="{4A88D659-4C13-44B6-A2BE-41980A9F7671}"/>
+    <workbookView xWindow="4725" yWindow="4530" windowWidth="18075" windowHeight="8340" xr2:uid="{4A88D659-4C13-44B6-A2BE-41980A9F7671}"/>
   </bookViews>
   <sheets>
     <sheet name="Actor_RobotObj_01" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
debug [Kinematics] fix coordinate over rotation.
</commit_message>
<xml_diff>
--- a/Actor_RobotObj_01.xlsx
+++ b/Actor_RobotObj_01.xlsx
@@ -5,29 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\waltz\Documents\CppProjects\GitManagements\QuantumCoreRobotRenew\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\CppGames\GitManagements\QuantumCoreFighterReMake\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{6736FA47-5E9A-4F07-8CDF-D36A6B0B9547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{872D9593-5224-4A07-B46B-1D87A66FC699}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4725" yWindow="4530" windowWidth="18075" windowHeight="8340" xr2:uid="{4A88D659-4C13-44B6-A2BE-41980A9F7671}"/>
+    <workbookView xWindow="564" yWindow="672" windowWidth="21336" windowHeight="8880" xr2:uid="{4A88D659-4C13-44B6-A2BE-41980A9F7671}"/>
   </bookViews>
   <sheets>
     <sheet name="Actor_RobotObj_01" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -983,25 +974,25 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomLeft" activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
     <col min="2" max="2" width="12.5" customWidth="1"/>
     <col min="3" max="3" width="5" customWidth="1"/>
     <col min="4" max="4" width="12.5" customWidth="1"/>
-    <col min="5" max="7" width="4.25" customWidth="1"/>
-    <col min="8" max="20" width="4.375" customWidth="1"/>
+    <col min="5" max="7" width="4.19921875" customWidth="1"/>
+    <col min="8" max="20" width="4.3984375" customWidth="1"/>
     <col min="22" max="22" width="12.5" customWidth="1"/>
-    <col min="23" max="25" width="4.25" customWidth="1"/>
-    <col min="26" max="29" width="4.375" customWidth="1"/>
-    <col min="30" max="30" width="7.625" customWidth="1"/>
-    <col min="31" max="31" width="30.875" customWidth="1"/>
+    <col min="23" max="25" width="4.19921875" customWidth="1"/>
+    <col min="26" max="29" width="4.3984375" customWidth="1"/>
+    <col min="30" max="30" width="7.59765625" customWidth="1"/>
+    <col min="31" max="31" width="30.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
@@ -1052,7 +1043,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A2" s="41" t="s">
         <v>0</v>
       </c>
@@ -1111,7 +1102,7 @@
       </c>
       <c r="AE2" s="32"/>
     </row>
-    <row r="3" spans="1:31" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:31" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A3" s="22"/>
       <c r="B3" s="23"/>
       <c r="C3" s="24"/>
@@ -1186,7 +1177,7 @@
       <c r="AD3" s="25"/>
       <c r="AE3" s="25"/>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -1261,10 +1252,10 @@
         <v>0</v>
       </c>
       <c r="Z4" s="20">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="3">
         <v>1</v>
-      </c>
-      <c r="AA4" s="3">
-        <v>0</v>
       </c>
       <c r="AB4" s="3">
         <v>0</v>
@@ -1277,7 +1268,7 @@
       </c>
       <c r="AE4" s="21"/>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A5" s="2">
         <v>2</v>
       </c>
@@ -1352,10 +1343,10 @@
         <v>0</v>
       </c>
       <c r="Z5" s="20">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="3">
         <v>1</v>
-      </c>
-      <c r="AA5" s="3">
-        <v>0</v>
       </c>
       <c r="AB5" s="3">
         <v>0</v>
@@ -1368,7 +1359,7 @@
       </c>
       <c r="AE5" s="8"/>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A6" s="2">
         <v>3</v>
       </c>
@@ -1443,10 +1434,10 @@
         <v>0</v>
       </c>
       <c r="Z6" s="20">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="3">
         <v>1</v>
-      </c>
-      <c r="AA6" s="3">
-        <v>0</v>
       </c>
       <c r="AB6" s="3">
         <v>0</v>
@@ -1459,7 +1450,7 @@
       </c>
       <c r="AE6" s="8"/>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A7" s="2">
         <v>4</v>
       </c>
@@ -1534,10 +1525,10 @@
         <v>0</v>
       </c>
       <c r="Z7" s="20">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="3">
         <v>1</v>
-      </c>
-      <c r="AA7" s="3">
-        <v>0</v>
       </c>
       <c r="AB7" s="3">
         <v>0</v>
@@ -1550,7 +1541,7 @@
       </c>
       <c r="AE7" s="8"/>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A8" s="2">
         <v>5</v>
       </c>
@@ -1625,10 +1616,10 @@
         <v>0</v>
       </c>
       <c r="Z8" s="20">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="3">
         <v>1</v>
-      </c>
-      <c r="AA8" s="3">
-        <v>0</v>
       </c>
       <c r="AB8" s="3">
         <v>0</v>
@@ -1641,7 +1632,7 @@
       </c>
       <c r="AE8" s="8"/>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A9" s="2">
         <v>6</v>
       </c>
@@ -1716,10 +1707,10 @@
         <v>0</v>
       </c>
       <c r="Z9" s="20">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="3">
         <v>1</v>
-      </c>
-      <c r="AA9" s="3">
-        <v>0</v>
       </c>
       <c r="AB9" s="3">
         <v>0</v>
@@ -1732,7 +1723,7 @@
       </c>
       <c r="AE9" s="8"/>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A10" s="2"/>
       <c r="B10" s="6"/>
       <c r="C10" s="7"/>
@@ -1765,7 +1756,7 @@
       <c r="AD10" s="8"/>
       <c r="AE10" s="8"/>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A11" s="2"/>
       <c r="B11" s="6"/>
       <c r="C11" s="7"/>
@@ -1798,7 +1789,7 @@
       <c r="AD11" s="8"/>
       <c r="AE11" s="8"/>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A12" s="2"/>
       <c r="B12" s="6"/>
       <c r="C12" s="7"/>
@@ -1831,7 +1822,7 @@
       <c r="AD12" s="8"/>
       <c r="AE12" s="8"/>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A13" s="2"/>
       <c r="B13" s="6"/>
       <c r="C13" s="7"/>
@@ -1864,7 +1855,7 @@
       <c r="AD13" s="8"/>
       <c r="AE13" s="8"/>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A14" s="2"/>
       <c r="B14" s="6"/>
       <c r="C14" s="7"/>
@@ -1897,7 +1888,7 @@
       <c r="AD14" s="8"/>
       <c r="AE14" s="8"/>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A15" s="2"/>
       <c r="B15" s="6"/>
       <c r="C15" s="7"/>
@@ -1930,7 +1921,7 @@
       <c r="AD15" s="8"/>
       <c r="AE15" s="8"/>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A16" s="2"/>
       <c r="B16" s="6"/>
       <c r="C16" s="7"/>
@@ -1963,7 +1954,7 @@
       <c r="AD16" s="8"/>
       <c r="AE16" s="8"/>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A17" s="2"/>
       <c r="B17" s="6"/>
       <c r="C17" s="7"/>
@@ -1996,7 +1987,7 @@
       <c r="AD17" s="8"/>
       <c r="AE17" s="8"/>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A18" s="2"/>
       <c r="B18" s="6"/>
       <c r="C18" s="7"/>
@@ -2029,7 +2020,7 @@
       <c r="AD18" s="8"/>
       <c r="AE18" s="8"/>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A19" s="2"/>
       <c r="B19" s="6"/>
       <c r="C19" s="7"/>
@@ -2062,7 +2053,7 @@
       <c r="AD19" s="8"/>
       <c r="AE19" s="8"/>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A20" s="2"/>
       <c r="B20" s="6"/>
       <c r="C20" s="7"/>
@@ -2095,7 +2086,7 @@
       <c r="AD20" s="8"/>
       <c r="AE20" s="8"/>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A21" s="2"/>
       <c r="B21" s="6"/>
       <c r="C21" s="7"/>
@@ -2128,7 +2119,7 @@
       <c r="AD21" s="8"/>
       <c r="AE21" s="8"/>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A22" s="2"/>
       <c r="B22" s="6"/>
       <c r="C22" s="7"/>
@@ -2161,7 +2152,7 @@
       <c r="AD22" s="8"/>
       <c r="AE22" s="8"/>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A23" s="2"/>
       <c r="B23" s="6"/>
       <c r="C23" s="7"/>
@@ -2194,7 +2185,7 @@
       <c r="AD23" s="8"/>
       <c r="AE23" s="8"/>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A24" s="2"/>
       <c r="B24" s="6"/>
       <c r="C24" s="7"/>
@@ -2227,7 +2218,7 @@
       <c r="AD24" s="8"/>
       <c r="AE24" s="8"/>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A25" s="2"/>
       <c r="B25" s="6"/>
       <c r="C25" s="7"/>
@@ -2260,7 +2251,7 @@
       <c r="AD25" s="8"/>
       <c r="AE25" s="8"/>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A26" s="2"/>
       <c r="B26" s="6"/>
       <c r="C26" s="7"/>
@@ -2293,7 +2284,7 @@
       <c r="AD26" s="8"/>
       <c r="AE26" s="8"/>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A27" s="2"/>
       <c r="B27" s="6"/>
       <c r="C27" s="7"/>
@@ -2326,7 +2317,7 @@
       <c r="AD27" s="8"/>
       <c r="AE27" s="8"/>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A28" s="2"/>
       <c r="B28" s="6"/>
       <c r="C28" s="7"/>
@@ -2359,7 +2350,7 @@
       <c r="AD28" s="8"/>
       <c r="AE28" s="8"/>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A29" s="2"/>
       <c r="B29" s="6"/>
       <c r="C29" s="7"/>
@@ -2392,7 +2383,7 @@
       <c r="AD29" s="8"/>
       <c r="AE29" s="8"/>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A30" s="2"/>
       <c r="B30" s="6"/>
       <c r="C30" s="7"/>
@@ -2425,7 +2416,7 @@
       <c r="AD30" s="8"/>
       <c r="AE30" s="8"/>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A31" s="2"/>
       <c r="B31" s="6"/>
       <c r="C31" s="7"/>
@@ -2458,7 +2449,7 @@
       <c r="AD31" s="8"/>
       <c r="AE31" s="8"/>
     </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A32" s="2"/>
       <c r="B32" s="6"/>
       <c r="C32" s="7"/>
@@ -2491,7 +2482,7 @@
       <c r="AD32" s="8"/>
       <c r="AE32" s="8"/>
     </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A33" s="2"/>
       <c r="B33" s="6"/>
       <c r="C33" s="7"/>
@@ -2524,7 +2515,7 @@
       <c r="AD33" s="8"/>
       <c r="AE33" s="8"/>
     </row>
-    <row r="34" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A34" s="2"/>
       <c r="B34" s="6"/>
       <c r="C34" s="7"/>
@@ -2557,7 +2548,7 @@
       <c r="AD34" s="8"/>
       <c r="AE34" s="8"/>
     </row>
-    <row r="35" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A35" s="2"/>
       <c r="B35" s="6"/>
       <c r="C35" s="7"/>
@@ -2590,7 +2581,7 @@
       <c r="AD35" s="8"/>
       <c r="AE35" s="8"/>
     </row>
-    <row r="36" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A36" s="2"/>
       <c r="B36" s="6"/>
       <c r="C36" s="7"/>
@@ -2623,7 +2614,7 @@
       <c r="AD36" s="8"/>
       <c r="AE36" s="8"/>
     </row>
-    <row r="37" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A37" s="2"/>
       <c r="B37" s="6"/>
       <c r="C37" s="7"/>
@@ -2656,7 +2647,7 @@
       <c r="AD37" s="8"/>
       <c r="AE37" s="8"/>
     </row>
-    <row r="38" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A38" s="2"/>
       <c r="B38" s="6"/>
       <c r="C38" s="7"/>
@@ -2689,7 +2680,7 @@
       <c r="AD38" s="8"/>
       <c r="AE38" s="8"/>
     </row>
-    <row r="39" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A39" s="2"/>
       <c r="B39" s="6"/>
       <c r="C39" s="7"/>
@@ -2722,7 +2713,7 @@
       <c r="AD39" s="8"/>
       <c r="AE39" s="8"/>
     </row>
-    <row r="40" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A40" s="2"/>
       <c r="B40" s="6"/>
       <c r="C40" s="7"/>
@@ -2755,7 +2746,7 @@
       <c r="AD40" s="8"/>
       <c r="AE40" s="8"/>
     </row>
-    <row r="41" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A41" s="2"/>
       <c r="B41" s="6"/>
       <c r="C41" s="7"/>
@@ -2788,7 +2779,7 @@
       <c r="AD41" s="8"/>
       <c r="AE41" s="8"/>
     </row>
-    <row r="42" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A42" s="2"/>
       <c r="B42" s="6"/>
       <c r="C42" s="7"/>
@@ -2821,7 +2812,7 @@
       <c r="AD42" s="8"/>
       <c r="AE42" s="8"/>
     </row>
-    <row r="43" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A43" s="2"/>
       <c r="B43" s="6"/>
       <c r="C43" s="7"/>
@@ -2854,7 +2845,7 @@
       <c r="AD43" s="8"/>
       <c r="AE43" s="8"/>
     </row>
-    <row r="44" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A44" s="2"/>
       <c r="B44" s="6"/>
       <c r="C44" s="7"/>
@@ -2887,7 +2878,7 @@
       <c r="AD44" s="8"/>
       <c r="AE44" s="8"/>
     </row>
-    <row r="45" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A45" s="2"/>
       <c r="B45" s="6"/>
       <c r="C45" s="7"/>
@@ -2920,7 +2911,7 @@
       <c r="AD45" s="8"/>
       <c r="AE45" s="8"/>
     </row>
-    <row r="46" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A46" s="2"/>
       <c r="B46" s="6"/>
       <c r="C46" s="7"/>
@@ -2953,7 +2944,7 @@
       <c r="AD46" s="8"/>
       <c r="AE46" s="8"/>
     </row>
-    <row r="47" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A47" s="2"/>
       <c r="B47" s="6"/>
       <c r="C47" s="7"/>
@@ -2986,7 +2977,7 @@
       <c r="AD47" s="8"/>
       <c r="AE47" s="8"/>
     </row>
-    <row r="48" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A48" s="2"/>
       <c r="B48" s="6"/>
       <c r="C48" s="7"/>
@@ -3019,7 +3010,7 @@
       <c r="AD48" s="8"/>
       <c r="AE48" s="8"/>
     </row>
-    <row r="49" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A49" s="2"/>
       <c r="B49" s="6"/>
       <c r="C49" s="7"/>
@@ -3052,7 +3043,7 @@
       <c r="AD49" s="8"/>
       <c r="AE49" s="8"/>
     </row>
-    <row r="50" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A50" s="2"/>
       <c r="B50" s="6"/>
       <c r="C50" s="7"/>
@@ -3085,7 +3076,7 @@
       <c r="AD50" s="8"/>
       <c r="AE50" s="8"/>
     </row>
-    <row r="51" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A51" s="2"/>
       <c r="B51" s="6"/>
       <c r="C51" s="7"/>
@@ -3118,7 +3109,7 @@
       <c r="AD51" s="8"/>
       <c r="AE51" s="8"/>
     </row>
-    <row r="52" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A52" s="2"/>
       <c r="B52" s="6"/>
       <c r="C52" s="7"/>
@@ -3151,7 +3142,7 @@
       <c r="AD52" s="8"/>
       <c r="AE52" s="8"/>
     </row>
-    <row r="53" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A53" s="2"/>
       <c r="B53" s="6"/>
       <c r="C53" s="7"/>
@@ -3184,7 +3175,7 @@
       <c r="AD53" s="8"/>
       <c r="AE53" s="8"/>
     </row>
-    <row r="54" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A54" s="2"/>
       <c r="B54" s="6"/>
       <c r="C54" s="7"/>
@@ -3217,7 +3208,7 @@
       <c r="AD54" s="8"/>
       <c r="AE54" s="8"/>
     </row>
-    <row r="55" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A55" s="2"/>
       <c r="B55" s="6"/>
       <c r="C55" s="7"/>
@@ -3250,7 +3241,7 @@
       <c r="AD55" s="8"/>
       <c r="AE55" s="8"/>
     </row>
-    <row r="56" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A56" s="2"/>
       <c r="B56" s="6"/>
       <c r="C56" s="7"/>
@@ -3283,7 +3274,7 @@
       <c r="AD56" s="8"/>
       <c r="AE56" s="8"/>
     </row>
-    <row r="57" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A57" s="2"/>
       <c r="B57" s="6"/>
       <c r="C57" s="7"/>
@@ -3316,7 +3307,7 @@
       <c r="AD57" s="8"/>
       <c r="AE57" s="8"/>
     </row>
-    <row r="58" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A58" s="2"/>
       <c r="B58" s="6"/>
       <c r="C58" s="7"/>
@@ -3349,7 +3340,7 @@
       <c r="AD58" s="8"/>
       <c r="AE58" s="8"/>
     </row>
-    <row r="59" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A59" s="2"/>
       <c r="B59" s="6"/>
       <c r="C59" s="7"/>
@@ -3382,7 +3373,7 @@
       <c r="AD59" s="8"/>
       <c r="AE59" s="8"/>
     </row>
-    <row r="60" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A60" s="2"/>
       <c r="B60" s="6"/>
       <c r="C60" s="7"/>
@@ -3415,7 +3406,7 @@
       <c r="AD60" s="8"/>
       <c r="AE60" s="8"/>
     </row>
-    <row r="61" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A61" s="2"/>
       <c r="B61" s="6"/>
       <c r="C61" s="7"/>
@@ -3448,7 +3439,7 @@
       <c r="AD61" s="8"/>
       <c r="AE61" s="8"/>
     </row>
-    <row r="62" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A62" s="2"/>
       <c r="B62" s="6"/>
       <c r="C62" s="7"/>
@@ -3481,7 +3472,7 @@
       <c r="AD62" s="8"/>
       <c r="AE62" s="8"/>
     </row>
-    <row r="63" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A63" s="2"/>
       <c r="B63" s="6"/>
       <c r="C63" s="7"/>
@@ -3514,7 +3505,7 @@
       <c r="AD63" s="8"/>
       <c r="AE63" s="8"/>
     </row>
-    <row r="64" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A64" s="2"/>
       <c r="B64" s="6"/>
       <c r="C64" s="7"/>
@@ -3547,7 +3538,7 @@
       <c r="AD64" s="8"/>
       <c r="AE64" s="8"/>
     </row>
-    <row r="65" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A65" s="2"/>
       <c r="B65" s="6"/>
       <c r="C65" s="7"/>
@@ -3580,7 +3571,7 @@
       <c r="AD65" s="8"/>
       <c r="AE65" s="8"/>
     </row>
-    <row r="66" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A66" s="2"/>
       <c r="B66" s="6"/>
       <c r="C66" s="7"/>
@@ -3613,7 +3604,7 @@
       <c r="AD66" s="8"/>
       <c r="AE66" s="8"/>
     </row>
-    <row r="67" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A67" s="2"/>
       <c r="B67" s="6"/>
       <c r="C67" s="7"/>
@@ -3646,7 +3637,7 @@
       <c r="AD67" s="8"/>
       <c r="AE67" s="8"/>
     </row>
-    <row r="68" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A68" s="2"/>
       <c r="B68" s="6"/>
       <c r="C68" s="7"/>
@@ -3679,7 +3670,7 @@
       <c r="AD68" s="8"/>
       <c r="AE68" s="8"/>
     </row>
-    <row r="69" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A69" s="2"/>
       <c r="B69" s="6"/>
       <c r="C69" s="7"/>
@@ -3712,7 +3703,7 @@
       <c r="AD69" s="8"/>
       <c r="AE69" s="8"/>
     </row>
-    <row r="70" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A70" s="2"/>
       <c r="B70" s="6"/>
       <c r="C70" s="7"/>
@@ -3745,7 +3736,7 @@
       <c r="AD70" s="8"/>
       <c r="AE70" s="8"/>
     </row>
-    <row r="71" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A71" s="2"/>
       <c r="B71" s="6"/>
       <c r="C71" s="7"/>
@@ -3778,7 +3769,7 @@
       <c r="AD71" s="8"/>
       <c r="AE71" s="8"/>
     </row>
-    <row r="72" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A72" s="2"/>
       <c r="B72" s="6"/>
       <c r="C72" s="7"/>
@@ -3811,7 +3802,7 @@
       <c r="AD72" s="8"/>
       <c r="AE72" s="8"/>
     </row>
-    <row r="73" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A73" s="2"/>
       <c r="B73" s="6"/>
       <c r="C73" s="7"/>
@@ -3844,7 +3835,7 @@
       <c r="AD73" s="8"/>
       <c r="AE73" s="8"/>
     </row>
-    <row r="74" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A74" s="2"/>
       <c r="B74" s="6"/>
       <c r="C74" s="7"/>
@@ -3877,7 +3868,7 @@
       <c r="AD74" s="8"/>
       <c r="AE74" s="8"/>
     </row>
-    <row r="75" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A75" s="2"/>
       <c r="B75" s="6"/>
       <c r="C75" s="7"/>
@@ -3910,7 +3901,7 @@
       <c r="AD75" s="8"/>
       <c r="AE75" s="8"/>
     </row>
-    <row r="76" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A76" s="2"/>
       <c r="B76" s="6"/>
       <c r="C76" s="7"/>
@@ -3943,7 +3934,7 @@
       <c r="AD76" s="8"/>
       <c r="AE76" s="8"/>
     </row>
-    <row r="77" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A77" s="2"/>
       <c r="B77" s="6"/>
       <c r="C77" s="7"/>
@@ -3976,7 +3967,7 @@
       <c r="AD77" s="8"/>
       <c r="AE77" s="8"/>
     </row>
-    <row r="78" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A78" s="2"/>
       <c r="B78" s="6"/>
       <c r="C78" s="7"/>
@@ -4009,7 +4000,7 @@
       <c r="AD78" s="8"/>
       <c r="AE78" s="8"/>
     </row>
-    <row r="79" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A79" s="2"/>
       <c r="B79" s="6"/>
       <c r="C79" s="7"/>
@@ -4042,7 +4033,7 @@
       <c r="AD79" s="8"/>
       <c r="AE79" s="8"/>
     </row>
-    <row r="80" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A80" s="2"/>
       <c r="B80" s="6"/>
       <c r="C80" s="7"/>
@@ -4075,7 +4066,7 @@
       <c r="AD80" s="8"/>
       <c r="AE80" s="8"/>
     </row>
-    <row r="81" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A81" s="2"/>
       <c r="B81" s="6"/>
       <c r="C81" s="7"/>
@@ -4108,7 +4099,7 @@
       <c r="AD81" s="8"/>
       <c r="AE81" s="8"/>
     </row>
-    <row r="82" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A82" s="2"/>
       <c r="B82" s="6"/>
       <c r="C82" s="7"/>
@@ -4141,7 +4132,7 @@
       <c r="AD82" s="8"/>
       <c r="AE82" s="8"/>
     </row>
-    <row r="83" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A83" s="2"/>
       <c r="B83" s="6"/>
       <c r="C83" s="7"/>
@@ -4174,7 +4165,7 @@
       <c r="AD83" s="8"/>
       <c r="AE83" s="8"/>
     </row>
-    <row r="84" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A84" s="2"/>
       <c r="B84" s="6"/>
       <c r="C84" s="7"/>
@@ -4207,7 +4198,7 @@
       <c r="AD84" s="8"/>
       <c r="AE84" s="8"/>
     </row>
-    <row r="85" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A85" s="2"/>
       <c r="B85" s="6"/>
       <c r="C85" s="7"/>
@@ -4240,7 +4231,7 @@
       <c r="AD85" s="8"/>
       <c r="AE85" s="8"/>
     </row>
-    <row r="86" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A86" s="2"/>
       <c r="B86" s="6"/>
       <c r="C86" s="7"/>
@@ -4273,7 +4264,7 @@
       <c r="AD86" s="8"/>
       <c r="AE86" s="8"/>
     </row>
-    <row r="87" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A87" s="2"/>
       <c r="B87" s="6"/>
       <c r="C87" s="7"/>
@@ -4306,7 +4297,7 @@
       <c r="AD87" s="8"/>
       <c r="AE87" s="8"/>
     </row>
-    <row r="88" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A88" s="2"/>
       <c r="B88" s="6"/>
       <c r="C88" s="7"/>
@@ -4339,7 +4330,7 @@
       <c r="AD88" s="8"/>
       <c r="AE88" s="8"/>
     </row>
-    <row r="89" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A89" s="2"/>
       <c r="B89" s="6"/>
       <c r="C89" s="7"/>
@@ -4372,7 +4363,7 @@
       <c r="AD89" s="8"/>
       <c r="AE89" s="8"/>
     </row>
-    <row r="90" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A90" s="2"/>
       <c r="B90" s="6"/>
       <c r="C90" s="7"/>
@@ -4405,7 +4396,7 @@
       <c r="AD90" s="8"/>
       <c r="AE90" s="8"/>
     </row>
-    <row r="91" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A91" s="2"/>
       <c r="B91" s="6"/>
       <c r="C91" s="7"/>
@@ -4438,7 +4429,7 @@
       <c r="AD91" s="8"/>
       <c r="AE91" s="8"/>
     </row>
-    <row r="92" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A92" s="2"/>
       <c r="B92" s="6"/>
       <c r="C92" s="7"/>
@@ -4471,7 +4462,7 @@
       <c r="AD92" s="8"/>
       <c r="AE92" s="8"/>
     </row>
-    <row r="93" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A93" s="2"/>
       <c r="B93" s="6"/>
       <c r="C93" s="7"/>
@@ -4504,7 +4495,7 @@
       <c r="AD93" s="8"/>
       <c r="AE93" s="8"/>
     </row>
-    <row r="94" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A94" s="2"/>
       <c r="B94" s="6"/>
       <c r="C94" s="7"/>
@@ -4537,7 +4528,7 @@
       <c r="AD94" s="8"/>
       <c r="AE94" s="8"/>
     </row>
-    <row r="95" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A95" s="2"/>
       <c r="B95" s="6"/>
       <c r="C95" s="7"/>
@@ -4570,7 +4561,7 @@
       <c r="AD95" s="8"/>
       <c r="AE95" s="8"/>
     </row>
-    <row r="96" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A96" s="2"/>
       <c r="B96" s="6"/>
       <c r="C96" s="7"/>
@@ -4603,7 +4594,7 @@
       <c r="AD96" s="8"/>
       <c r="AE96" s="8"/>
     </row>
-    <row r="97" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A97" s="2"/>
       <c r="B97" s="6"/>
       <c r="C97" s="7"/>
@@ -4636,7 +4627,7 @@
       <c r="AD97" s="8"/>
       <c r="AE97" s="8"/>
     </row>
-    <row r="98" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A98" s="2"/>
       <c r="B98" s="6"/>
       <c r="C98" s="7"/>
@@ -4669,7 +4660,7 @@
       <c r="AD98" s="8"/>
       <c r="AE98" s="8"/>
     </row>
-    <row r="99" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A99" s="2"/>
       <c r="B99" s="6"/>
       <c r="C99" s="7"/>
@@ -4702,7 +4693,7 @@
       <c r="AD99" s="8"/>
       <c r="AE99" s="8"/>
     </row>
-    <row r="100" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A100" s="2"/>
       <c r="B100" s="6"/>
       <c r="C100" s="7"/>
@@ -4735,7 +4726,7 @@
       <c r="AD100" s="8"/>
       <c r="AE100" s="8"/>
     </row>
-    <row r="101" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A101" s="2"/>
       <c r="B101" s="6"/>
       <c r="C101" s="7"/>
@@ -4768,7 +4759,7 @@
       <c r="AD101" s="8"/>
       <c r="AE101" s="8"/>
     </row>
-    <row r="102" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="102" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A102" s="2"/>
       <c r="B102" s="6"/>
       <c r="C102" s="7"/>
@@ -4801,7 +4792,7 @@
       <c r="AD102" s="8"/>
       <c r="AE102" s="8"/>
     </row>
-    <row r="103" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="103" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A103" s="27"/>
       <c r="B103" s="28"/>
       <c r="C103" s="29"/>
@@ -4834,7 +4825,7 @@
       <c r="AD103" s="30"/>
       <c r="AE103" s="30"/>
     </row>
-    <row r="104" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A104" s="31"/>
       <c r="B104" s="31"/>
       <c r="C104" s="31"/>

</xml_diff>

<commit_message>
debug :[Kinematics] fixed! next mission : IK
</commit_message>
<xml_diff>
--- a/Actor_RobotObj_01.xlsx
+++ b/Actor_RobotObj_01.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\CppGames\GitManagements\QuantumCoreFighterReMake\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\waltz\Documents\CppProjects\GitManagements\QuantumCoreRobotReMake\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{872D9593-5224-4A07-B46B-1D87A66FC699}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{0F5E2987-6B49-4D52-A2D2-BD505D59BEF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="564" yWindow="672" windowWidth="21336" windowHeight="8880" xr2:uid="{4A88D659-4C13-44B6-A2BE-41980A9F7671}"/>
+    <workbookView xWindow="990" yWindow="3645" windowWidth="19740" windowHeight="7440" xr2:uid="{4A88D659-4C13-44B6-A2BE-41980A9F7671}"/>
   </bookViews>
   <sheets>
     <sheet name="Actor_RobotObj_01" sheetId="1" r:id="rId1"/>
@@ -974,25 +974,25 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L6" sqref="L6"/>
+      <selection pane="bottomLeft" activeCell="W4" sqref="W4:W9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
     <col min="2" max="2" width="12.5" customWidth="1"/>
     <col min="3" max="3" width="5" customWidth="1"/>
     <col min="4" max="4" width="12.5" customWidth="1"/>
-    <col min="5" max="7" width="4.19921875" customWidth="1"/>
-    <col min="8" max="20" width="4.3984375" customWidth="1"/>
+    <col min="5" max="7" width="4.25" customWidth="1"/>
+    <col min="8" max="20" width="4.375" customWidth="1"/>
     <col min="22" max="22" width="12.5" customWidth="1"/>
-    <col min="23" max="25" width="4.19921875" customWidth="1"/>
-    <col min="26" max="29" width="4.3984375" customWidth="1"/>
-    <col min="30" max="30" width="7.59765625" customWidth="1"/>
-    <col min="31" max="31" width="30.8984375" customWidth="1"/>
+    <col min="23" max="25" width="4.25" customWidth="1"/>
+    <col min="26" max="29" width="4.375" customWidth="1"/>
+    <col min="30" max="30" width="7.625" customWidth="1"/>
+    <col min="31" max="31" width="30.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
@@ -1043,7 +1043,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A2" s="41" t="s">
         <v>0</v>
       </c>
@@ -1102,7 +1102,7 @@
       </c>
       <c r="AE2" s="32"/>
     </row>
-    <row r="3" spans="1:31" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:31" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="22"/>
       <c r="B3" s="23"/>
       <c r="C3" s="24"/>
@@ -1177,7 +1177,7 @@
       <c r="AD3" s="25"/>
       <c r="AE3" s="25"/>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -1243,7 +1243,7 @@
       </c>
       <c r="V4" s="21"/>
       <c r="W4" s="20">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="X4" s="3">
         <v>0</v>
@@ -1252,23 +1252,23 @@
         <v>0</v>
       </c>
       <c r="Z4" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA4" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB4" s="3">
         <v>0</v>
       </c>
       <c r="AC4" s="21">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="AD4" s="21">
         <v>1</v>
       </c>
       <c r="AE4" s="21"/>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A5" s="2">
         <v>2</v>
       </c>
@@ -1334,7 +1334,7 @@
       </c>
       <c r="V5" s="8"/>
       <c r="W5" s="7">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="X5" s="2">
         <v>0</v>
@@ -1343,23 +1343,23 @@
         <v>0</v>
       </c>
       <c r="Z5" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA5" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB5" s="3">
         <v>0</v>
       </c>
       <c r="AC5" s="21">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="AD5" s="21">
         <v>1</v>
       </c>
       <c r="AE5" s="8"/>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A6" s="2">
         <v>3</v>
       </c>
@@ -1425,7 +1425,7 @@
       </c>
       <c r="V6" s="8"/>
       <c r="W6" s="20">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="X6" s="3">
         <v>0</v>
@@ -1434,23 +1434,23 @@
         <v>0</v>
       </c>
       <c r="Z6" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA6" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB6" s="3">
         <v>0</v>
       </c>
       <c r="AC6" s="21">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="AD6" s="21">
         <v>1</v>
       </c>
       <c r="AE6" s="8"/>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A7" s="2">
         <v>4</v>
       </c>
@@ -1516,7 +1516,7 @@
       </c>
       <c r="V7" s="8"/>
       <c r="W7" s="7">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="X7" s="2">
         <v>0</v>
@@ -1525,23 +1525,23 @@
         <v>0</v>
       </c>
       <c r="Z7" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA7" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB7" s="3">
         <v>0</v>
       </c>
       <c r="AC7" s="21">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="AD7" s="21">
         <v>1</v>
       </c>
       <c r="AE7" s="8"/>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A8" s="2">
         <v>5</v>
       </c>
@@ -1607,7 +1607,7 @@
       </c>
       <c r="V8" s="8"/>
       <c r="W8" s="20">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="X8" s="3">
         <v>0</v>
@@ -1616,23 +1616,23 @@
         <v>0</v>
       </c>
       <c r="Z8" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA8" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB8" s="3">
         <v>0</v>
       </c>
       <c r="AC8" s="21">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="AD8" s="8">
         <v>1</v>
       </c>
       <c r="AE8" s="8"/>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A9" s="2">
         <v>6</v>
       </c>
@@ -1698,7 +1698,7 @@
       </c>
       <c r="V9" s="8"/>
       <c r="W9" s="7">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="X9" s="2">
         <v>0</v>
@@ -1707,23 +1707,23 @@
         <v>0</v>
       </c>
       <c r="Z9" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA9" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB9" s="3">
         <v>0</v>
       </c>
       <c r="AC9" s="21">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="AD9" s="8">
         <v>1</v>
       </c>
       <c r="AE9" s="8"/>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A10" s="2"/>
       <c r="B10" s="6"/>
       <c r="C10" s="7"/>
@@ -1756,7 +1756,7 @@
       <c r="AD10" s="8"/>
       <c r="AE10" s="8"/>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A11" s="2"/>
       <c r="B11" s="6"/>
       <c r="C11" s="7"/>
@@ -1789,7 +1789,7 @@
       <c r="AD11" s="8"/>
       <c r="AE11" s="8"/>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A12" s="2"/>
       <c r="B12" s="6"/>
       <c r="C12" s="7"/>
@@ -1822,7 +1822,7 @@
       <c r="AD12" s="8"/>
       <c r="AE12" s="8"/>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A13" s="2"/>
       <c r="B13" s="6"/>
       <c r="C13" s="7"/>
@@ -1855,7 +1855,7 @@
       <c r="AD13" s="8"/>
       <c r="AE13" s="8"/>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A14" s="2"/>
       <c r="B14" s="6"/>
       <c r="C14" s="7"/>
@@ -1888,7 +1888,7 @@
       <c r="AD14" s="8"/>
       <c r="AE14" s="8"/>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A15" s="2"/>
       <c r="B15" s="6"/>
       <c r="C15" s="7"/>
@@ -1921,7 +1921,7 @@
       <c r="AD15" s="8"/>
       <c r="AE15" s="8"/>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A16" s="2"/>
       <c r="B16" s="6"/>
       <c r="C16" s="7"/>
@@ -1954,7 +1954,7 @@
       <c r="AD16" s="8"/>
       <c r="AE16" s="8"/>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A17" s="2"/>
       <c r="B17" s="6"/>
       <c r="C17" s="7"/>
@@ -1987,7 +1987,7 @@
       <c r="AD17" s="8"/>
       <c r="AE17" s="8"/>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A18" s="2"/>
       <c r="B18" s="6"/>
       <c r="C18" s="7"/>
@@ -2020,7 +2020,7 @@
       <c r="AD18" s="8"/>
       <c r="AE18" s="8"/>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A19" s="2"/>
       <c r="B19" s="6"/>
       <c r="C19" s="7"/>
@@ -2053,7 +2053,7 @@
       <c r="AD19" s="8"/>
       <c r="AE19" s="8"/>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A20" s="2"/>
       <c r="B20" s="6"/>
       <c r="C20" s="7"/>
@@ -2086,7 +2086,7 @@
       <c r="AD20" s="8"/>
       <c r="AE20" s="8"/>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A21" s="2"/>
       <c r="B21" s="6"/>
       <c r="C21" s="7"/>
@@ -2119,7 +2119,7 @@
       <c r="AD21" s="8"/>
       <c r="AE21" s="8"/>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A22" s="2"/>
       <c r="B22" s="6"/>
       <c r="C22" s="7"/>
@@ -2152,7 +2152,7 @@
       <c r="AD22" s="8"/>
       <c r="AE22" s="8"/>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A23" s="2"/>
       <c r="B23" s="6"/>
       <c r="C23" s="7"/>
@@ -2185,7 +2185,7 @@
       <c r="AD23" s="8"/>
       <c r="AE23" s="8"/>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A24" s="2"/>
       <c r="B24" s="6"/>
       <c r="C24" s="7"/>
@@ -2218,7 +2218,7 @@
       <c r="AD24" s="8"/>
       <c r="AE24" s="8"/>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A25" s="2"/>
       <c r="B25" s="6"/>
       <c r="C25" s="7"/>
@@ -2251,7 +2251,7 @@
       <c r="AD25" s="8"/>
       <c r="AE25" s="8"/>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A26" s="2"/>
       <c r="B26" s="6"/>
       <c r="C26" s="7"/>
@@ -2284,7 +2284,7 @@
       <c r="AD26" s="8"/>
       <c r="AE26" s="8"/>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A27" s="2"/>
       <c r="B27" s="6"/>
       <c r="C27" s="7"/>
@@ -2317,7 +2317,7 @@
       <c r="AD27" s="8"/>
       <c r="AE27" s="8"/>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A28" s="2"/>
       <c r="B28" s="6"/>
       <c r="C28" s="7"/>
@@ -2350,7 +2350,7 @@
       <c r="AD28" s="8"/>
       <c r="AE28" s="8"/>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A29" s="2"/>
       <c r="B29" s="6"/>
       <c r="C29" s="7"/>
@@ -2383,7 +2383,7 @@
       <c r="AD29" s="8"/>
       <c r="AE29" s="8"/>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A30" s="2"/>
       <c r="B30" s="6"/>
       <c r="C30" s="7"/>
@@ -2416,7 +2416,7 @@
       <c r="AD30" s="8"/>
       <c r="AE30" s="8"/>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A31" s="2"/>
       <c r="B31" s="6"/>
       <c r="C31" s="7"/>
@@ -2449,7 +2449,7 @@
       <c r="AD31" s="8"/>
       <c r="AE31" s="8"/>
     </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A32" s="2"/>
       <c r="B32" s="6"/>
       <c r="C32" s="7"/>
@@ -2482,7 +2482,7 @@
       <c r="AD32" s="8"/>
       <c r="AE32" s="8"/>
     </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A33" s="2"/>
       <c r="B33" s="6"/>
       <c r="C33" s="7"/>
@@ -2515,7 +2515,7 @@
       <c r="AD33" s="8"/>
       <c r="AE33" s="8"/>
     </row>
-    <row r="34" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A34" s="2"/>
       <c r="B34" s="6"/>
       <c r="C34" s="7"/>
@@ -2548,7 +2548,7 @@
       <c r="AD34" s="8"/>
       <c r="AE34" s="8"/>
     </row>
-    <row r="35" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A35" s="2"/>
       <c r="B35" s="6"/>
       <c r="C35" s="7"/>
@@ -2581,7 +2581,7 @@
       <c r="AD35" s="8"/>
       <c r="AE35" s="8"/>
     </row>
-    <row r="36" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A36" s="2"/>
       <c r="B36" s="6"/>
       <c r="C36" s="7"/>
@@ -2614,7 +2614,7 @@
       <c r="AD36" s="8"/>
       <c r="AE36" s="8"/>
     </row>
-    <row r="37" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A37" s="2"/>
       <c r="B37" s="6"/>
       <c r="C37" s="7"/>
@@ -2647,7 +2647,7 @@
       <c r="AD37" s="8"/>
       <c r="AE37" s="8"/>
     </row>
-    <row r="38" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A38" s="2"/>
       <c r="B38" s="6"/>
       <c r="C38" s="7"/>
@@ -2680,7 +2680,7 @@
       <c r="AD38" s="8"/>
       <c r="AE38" s="8"/>
     </row>
-    <row r="39" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A39" s="2"/>
       <c r="B39" s="6"/>
       <c r="C39" s="7"/>
@@ -2713,7 +2713,7 @@
       <c r="AD39" s="8"/>
       <c r="AE39" s="8"/>
     </row>
-    <row r="40" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A40" s="2"/>
       <c r="B40" s="6"/>
       <c r="C40" s="7"/>
@@ -2746,7 +2746,7 @@
       <c r="AD40" s="8"/>
       <c r="AE40" s="8"/>
     </row>
-    <row r="41" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A41" s="2"/>
       <c r="B41" s="6"/>
       <c r="C41" s="7"/>
@@ -2779,7 +2779,7 @@
       <c r="AD41" s="8"/>
       <c r="AE41" s="8"/>
     </row>
-    <row r="42" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A42" s="2"/>
       <c r="B42" s="6"/>
       <c r="C42" s="7"/>
@@ -2812,7 +2812,7 @@
       <c r="AD42" s="8"/>
       <c r="AE42" s="8"/>
     </row>
-    <row r="43" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A43" s="2"/>
       <c r="B43" s="6"/>
       <c r="C43" s="7"/>
@@ -2845,7 +2845,7 @@
       <c r="AD43" s="8"/>
       <c r="AE43" s="8"/>
     </row>
-    <row r="44" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A44" s="2"/>
       <c r="B44" s="6"/>
       <c r="C44" s="7"/>
@@ -2878,7 +2878,7 @@
       <c r="AD44" s="8"/>
       <c r="AE44" s="8"/>
     </row>
-    <row r="45" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A45" s="2"/>
       <c r="B45" s="6"/>
       <c r="C45" s="7"/>
@@ -2911,7 +2911,7 @@
       <c r="AD45" s="8"/>
       <c r="AE45" s="8"/>
     </row>
-    <row r="46" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A46" s="2"/>
       <c r="B46" s="6"/>
       <c r="C46" s="7"/>
@@ -2944,7 +2944,7 @@
       <c r="AD46" s="8"/>
       <c r="AE46" s="8"/>
     </row>
-    <row r="47" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A47" s="2"/>
       <c r="B47" s="6"/>
       <c r="C47" s="7"/>
@@ -2977,7 +2977,7 @@
       <c r="AD47" s="8"/>
       <c r="AE47" s="8"/>
     </row>
-    <row r="48" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A48" s="2"/>
       <c r="B48" s="6"/>
       <c r="C48" s="7"/>
@@ -3010,7 +3010,7 @@
       <c r="AD48" s="8"/>
       <c r="AE48" s="8"/>
     </row>
-    <row r="49" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A49" s="2"/>
       <c r="B49" s="6"/>
       <c r="C49" s="7"/>
@@ -3043,7 +3043,7 @@
       <c r="AD49" s="8"/>
       <c r="AE49" s="8"/>
     </row>
-    <row r="50" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A50" s="2"/>
       <c r="B50" s="6"/>
       <c r="C50" s="7"/>
@@ -3076,7 +3076,7 @@
       <c r="AD50" s="8"/>
       <c r="AE50" s="8"/>
     </row>
-    <row r="51" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A51" s="2"/>
       <c r="B51" s="6"/>
       <c r="C51" s="7"/>
@@ -3109,7 +3109,7 @@
       <c r="AD51" s="8"/>
       <c r="AE51" s="8"/>
     </row>
-    <row r="52" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A52" s="2"/>
       <c r="B52" s="6"/>
       <c r="C52" s="7"/>
@@ -3142,7 +3142,7 @@
       <c r="AD52" s="8"/>
       <c r="AE52" s="8"/>
     </row>
-    <row r="53" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A53" s="2"/>
       <c r="B53" s="6"/>
       <c r="C53" s="7"/>
@@ -3175,7 +3175,7 @@
       <c r="AD53" s="8"/>
       <c r="AE53" s="8"/>
     </row>
-    <row r="54" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A54" s="2"/>
       <c r="B54" s="6"/>
       <c r="C54" s="7"/>
@@ -3208,7 +3208,7 @@
       <c r="AD54" s="8"/>
       <c r="AE54" s="8"/>
     </row>
-    <row r="55" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A55" s="2"/>
       <c r="B55" s="6"/>
       <c r="C55" s="7"/>
@@ -3241,7 +3241,7 @@
       <c r="AD55" s="8"/>
       <c r="AE55" s="8"/>
     </row>
-    <row r="56" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A56" s="2"/>
       <c r="B56" s="6"/>
       <c r="C56" s="7"/>
@@ -3274,7 +3274,7 @@
       <c r="AD56" s="8"/>
       <c r="AE56" s="8"/>
     </row>
-    <row r="57" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A57" s="2"/>
       <c r="B57" s="6"/>
       <c r="C57" s="7"/>
@@ -3307,7 +3307,7 @@
       <c r="AD57" s="8"/>
       <c r="AE57" s="8"/>
     </row>
-    <row r="58" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A58" s="2"/>
       <c r="B58" s="6"/>
       <c r="C58" s="7"/>
@@ -3340,7 +3340,7 @@
       <c r="AD58" s="8"/>
       <c r="AE58" s="8"/>
     </row>
-    <row r="59" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A59" s="2"/>
       <c r="B59" s="6"/>
       <c r="C59" s="7"/>
@@ -3373,7 +3373,7 @@
       <c r="AD59" s="8"/>
       <c r="AE59" s="8"/>
     </row>
-    <row r="60" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A60" s="2"/>
       <c r="B60" s="6"/>
       <c r="C60" s="7"/>
@@ -3406,7 +3406,7 @@
       <c r="AD60" s="8"/>
       <c r="AE60" s="8"/>
     </row>
-    <row r="61" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A61" s="2"/>
       <c r="B61" s="6"/>
       <c r="C61" s="7"/>
@@ -3439,7 +3439,7 @@
       <c r="AD61" s="8"/>
       <c r="AE61" s="8"/>
     </row>
-    <row r="62" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A62" s="2"/>
       <c r="B62" s="6"/>
       <c r="C62" s="7"/>
@@ -3472,7 +3472,7 @@
       <c r="AD62" s="8"/>
       <c r="AE62" s="8"/>
     </row>
-    <row r="63" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A63" s="2"/>
       <c r="B63" s="6"/>
       <c r="C63" s="7"/>
@@ -3505,7 +3505,7 @@
       <c r="AD63" s="8"/>
       <c r="AE63" s="8"/>
     </row>
-    <row r="64" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A64" s="2"/>
       <c r="B64" s="6"/>
       <c r="C64" s="7"/>
@@ -3538,7 +3538,7 @@
       <c r="AD64" s="8"/>
       <c r="AE64" s="8"/>
     </row>
-    <row r="65" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A65" s="2"/>
       <c r="B65" s="6"/>
       <c r="C65" s="7"/>
@@ -3571,7 +3571,7 @@
       <c r="AD65" s="8"/>
       <c r="AE65" s="8"/>
     </row>
-    <row r="66" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A66" s="2"/>
       <c r="B66" s="6"/>
       <c r="C66" s="7"/>
@@ -3604,7 +3604,7 @@
       <c r="AD66" s="8"/>
       <c r="AE66" s="8"/>
     </row>
-    <row r="67" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A67" s="2"/>
       <c r="B67" s="6"/>
       <c r="C67" s="7"/>
@@ -3637,7 +3637,7 @@
       <c r="AD67" s="8"/>
       <c r="AE67" s="8"/>
     </row>
-    <row r="68" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A68" s="2"/>
       <c r="B68" s="6"/>
       <c r="C68" s="7"/>
@@ -3670,7 +3670,7 @@
       <c r="AD68" s="8"/>
       <c r="AE68" s="8"/>
     </row>
-    <row r="69" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A69" s="2"/>
       <c r="B69" s="6"/>
       <c r="C69" s="7"/>
@@ -3703,7 +3703,7 @@
       <c r="AD69" s="8"/>
       <c r="AE69" s="8"/>
     </row>
-    <row r="70" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A70" s="2"/>
       <c r="B70" s="6"/>
       <c r="C70" s="7"/>
@@ -3736,7 +3736,7 @@
       <c r="AD70" s="8"/>
       <c r="AE70" s="8"/>
     </row>
-    <row r="71" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A71" s="2"/>
       <c r="B71" s="6"/>
       <c r="C71" s="7"/>
@@ -3769,7 +3769,7 @@
       <c r="AD71" s="8"/>
       <c r="AE71" s="8"/>
     </row>
-    <row r="72" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A72" s="2"/>
       <c r="B72" s="6"/>
       <c r="C72" s="7"/>
@@ -3802,7 +3802,7 @@
       <c r="AD72" s="8"/>
       <c r="AE72" s="8"/>
     </row>
-    <row r="73" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A73" s="2"/>
       <c r="B73" s="6"/>
       <c r="C73" s="7"/>
@@ -3835,7 +3835,7 @@
       <c r="AD73" s="8"/>
       <c r="AE73" s="8"/>
     </row>
-    <row r="74" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A74" s="2"/>
       <c r="B74" s="6"/>
       <c r="C74" s="7"/>
@@ -3868,7 +3868,7 @@
       <c r="AD74" s="8"/>
       <c r="AE74" s="8"/>
     </row>
-    <row r="75" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A75" s="2"/>
       <c r="B75" s="6"/>
       <c r="C75" s="7"/>
@@ -3901,7 +3901,7 @@
       <c r="AD75" s="8"/>
       <c r="AE75" s="8"/>
     </row>
-    <row r="76" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A76" s="2"/>
       <c r="B76" s="6"/>
       <c r="C76" s="7"/>
@@ -3934,7 +3934,7 @@
       <c r="AD76" s="8"/>
       <c r="AE76" s="8"/>
     </row>
-    <row r="77" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A77" s="2"/>
       <c r="B77" s="6"/>
       <c r="C77" s="7"/>
@@ -3967,7 +3967,7 @@
       <c r="AD77" s="8"/>
       <c r="AE77" s="8"/>
     </row>
-    <row r="78" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A78" s="2"/>
       <c r="B78" s="6"/>
       <c r="C78" s="7"/>
@@ -4000,7 +4000,7 @@
       <c r="AD78" s="8"/>
       <c r="AE78" s="8"/>
     </row>
-    <row r="79" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A79" s="2"/>
       <c r="B79" s="6"/>
       <c r="C79" s="7"/>
@@ -4033,7 +4033,7 @@
       <c r="AD79" s="8"/>
       <c r="AE79" s="8"/>
     </row>
-    <row r="80" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A80" s="2"/>
       <c r="B80" s="6"/>
       <c r="C80" s="7"/>
@@ -4066,7 +4066,7 @@
       <c r="AD80" s="8"/>
       <c r="AE80" s="8"/>
     </row>
-    <row r="81" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A81" s="2"/>
       <c r="B81" s="6"/>
       <c r="C81" s="7"/>
@@ -4099,7 +4099,7 @@
       <c r="AD81" s="8"/>
       <c r="AE81" s="8"/>
     </row>
-    <row r="82" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A82" s="2"/>
       <c r="B82" s="6"/>
       <c r="C82" s="7"/>
@@ -4132,7 +4132,7 @@
       <c r="AD82" s="8"/>
       <c r="AE82" s="8"/>
     </row>
-    <row r="83" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A83" s="2"/>
       <c r="B83" s="6"/>
       <c r="C83" s="7"/>
@@ -4165,7 +4165,7 @@
       <c r="AD83" s="8"/>
       <c r="AE83" s="8"/>
     </row>
-    <row r="84" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A84" s="2"/>
       <c r="B84" s="6"/>
       <c r="C84" s="7"/>
@@ -4198,7 +4198,7 @@
       <c r="AD84" s="8"/>
       <c r="AE84" s="8"/>
     </row>
-    <row r="85" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A85" s="2"/>
       <c r="B85" s="6"/>
       <c r="C85" s="7"/>
@@ -4231,7 +4231,7 @@
       <c r="AD85" s="8"/>
       <c r="AE85" s="8"/>
     </row>
-    <row r="86" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A86" s="2"/>
       <c r="B86" s="6"/>
       <c r="C86" s="7"/>
@@ -4264,7 +4264,7 @@
       <c r="AD86" s="8"/>
       <c r="AE86" s="8"/>
     </row>
-    <row r="87" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A87" s="2"/>
       <c r="B87" s="6"/>
       <c r="C87" s="7"/>
@@ -4297,7 +4297,7 @@
       <c r="AD87" s="8"/>
       <c r="AE87" s="8"/>
     </row>
-    <row r="88" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A88" s="2"/>
       <c r="B88" s="6"/>
       <c r="C88" s="7"/>
@@ -4330,7 +4330,7 @@
       <c r="AD88" s="8"/>
       <c r="AE88" s="8"/>
     </row>
-    <row r="89" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A89" s="2"/>
       <c r="B89" s="6"/>
       <c r="C89" s="7"/>
@@ -4363,7 +4363,7 @@
       <c r="AD89" s="8"/>
       <c r="AE89" s="8"/>
     </row>
-    <row r="90" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A90" s="2"/>
       <c r="B90" s="6"/>
       <c r="C90" s="7"/>
@@ -4396,7 +4396,7 @@
       <c r="AD90" s="8"/>
       <c r="AE90" s="8"/>
     </row>
-    <row r="91" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A91" s="2"/>
       <c r="B91" s="6"/>
       <c r="C91" s="7"/>
@@ -4429,7 +4429,7 @@
       <c r="AD91" s="8"/>
       <c r="AE91" s="8"/>
     </row>
-    <row r="92" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A92" s="2"/>
       <c r="B92" s="6"/>
       <c r="C92" s="7"/>
@@ -4462,7 +4462,7 @@
       <c r="AD92" s="8"/>
       <c r="AE92" s="8"/>
     </row>
-    <row r="93" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A93" s="2"/>
       <c r="B93" s="6"/>
       <c r="C93" s="7"/>
@@ -4495,7 +4495,7 @@
       <c r="AD93" s="8"/>
       <c r="AE93" s="8"/>
     </row>
-    <row r="94" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A94" s="2"/>
       <c r="B94" s="6"/>
       <c r="C94" s="7"/>
@@ -4528,7 +4528,7 @@
       <c r="AD94" s="8"/>
       <c r="AE94" s="8"/>
     </row>
-    <row r="95" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A95" s="2"/>
       <c r="B95" s="6"/>
       <c r="C95" s="7"/>
@@ -4561,7 +4561,7 @@
       <c r="AD95" s="8"/>
       <c r="AE95" s="8"/>
     </row>
-    <row r="96" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A96" s="2"/>
       <c r="B96" s="6"/>
       <c r="C96" s="7"/>
@@ -4594,7 +4594,7 @@
       <c r="AD96" s="8"/>
       <c r="AE96" s="8"/>
     </row>
-    <row r="97" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A97" s="2"/>
       <c r="B97" s="6"/>
       <c r="C97" s="7"/>
@@ -4627,7 +4627,7 @@
       <c r="AD97" s="8"/>
       <c r="AE97" s="8"/>
     </row>
-    <row r="98" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A98" s="2"/>
       <c r="B98" s="6"/>
       <c r="C98" s="7"/>
@@ -4660,7 +4660,7 @@
       <c r="AD98" s="8"/>
       <c r="AE98" s="8"/>
     </row>
-    <row r="99" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A99" s="2"/>
       <c r="B99" s="6"/>
       <c r="C99" s="7"/>
@@ -4693,7 +4693,7 @@
       <c r="AD99" s="8"/>
       <c r="AE99" s="8"/>
     </row>
-    <row r="100" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A100" s="2"/>
       <c r="B100" s="6"/>
       <c r="C100" s="7"/>
@@ -4726,7 +4726,7 @@
       <c r="AD100" s="8"/>
       <c r="AE100" s="8"/>
     </row>
-    <row r="101" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A101" s="2"/>
       <c r="B101" s="6"/>
       <c r="C101" s="7"/>
@@ -4759,7 +4759,7 @@
       <c r="AD101" s="8"/>
       <c r="AE101" s="8"/>
     </row>
-    <row r="102" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A102" s="2"/>
       <c r="B102" s="6"/>
       <c r="C102" s="7"/>
@@ -4792,7 +4792,7 @@
       <c r="AD102" s="8"/>
       <c r="AE102" s="8"/>
     </row>
-    <row r="103" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A103" s="27"/>
       <c r="B103" s="28"/>
       <c r="C103" s="29"/>
@@ -4825,7 +4825,7 @@
       <c r="AD103" s="30"/>
       <c r="AE103" s="30"/>
     </row>
-    <row r="104" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A104" s="31"/>
       <c r="B104" s="31"/>
       <c r="C104" s="31"/>

</xml_diff>

<commit_message>
add : [InvKinametics] do IK construction (reed IK setting csv & create InvKinematics class -> set to Kinematics class )
</commit_message>
<xml_diff>
--- a/Actor_RobotObj_01.xlsx
+++ b/Actor_RobotObj_01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\waltz\Documents\CppProjects\GitManagements\QuantumCoreRobotReMake\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{0F5E2987-6B49-4D52-A2D2-BD505D59BEF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{C9554B95-70B5-4E00-9A3C-96780F06325F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="990" yWindow="3645" windowWidth="19740" windowHeight="7440" xr2:uid="{4A88D659-4C13-44B6-A2BE-41980A9F7671}"/>
+    <workbookView xWindow="-23535" yWindow="4905" windowWidth="17220" windowHeight="10980" xr2:uid="{4A88D659-4C13-44B6-A2BE-41980A9F7671}"/>
   </bookViews>
   <sheets>
     <sheet name="Actor_RobotObj_01" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="37">
   <si>
     <t>id</t>
     <phoneticPr fontId="1"/>
@@ -145,6 +145,30 @@
   </si>
   <si>
     <t>root</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>objEE01</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>obj6</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> IK object</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>target01</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>root</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>IK target</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -974,7 +998,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W4" sqref="W4:W9"/>
+      <selection pane="bottomLeft" activeCell="AC4" sqref="AC4:AC9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -1243,7 +1267,7 @@
       </c>
       <c r="V4" s="21"/>
       <c r="W4" s="20">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="X4" s="3">
         <v>0</v>
@@ -1261,7 +1285,7 @@
         <v>0</v>
       </c>
       <c r="AC4" s="21">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="AD4" s="21">
         <v>1</v>
@@ -1334,7 +1358,7 @@
       </c>
       <c r="V5" s="8"/>
       <c r="W5" s="7">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="X5" s="2">
         <v>0</v>
@@ -1352,7 +1376,7 @@
         <v>0</v>
       </c>
       <c r="AC5" s="21">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="AD5" s="21">
         <v>1</v>
@@ -1425,7 +1449,7 @@
       </c>
       <c r="V6" s="8"/>
       <c r="W6" s="20">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="X6" s="3">
         <v>0</v>
@@ -1443,7 +1467,7 @@
         <v>0</v>
       </c>
       <c r="AC6" s="21">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="AD6" s="21">
         <v>1</v>
@@ -1516,7 +1540,7 @@
       </c>
       <c r="V7" s="8"/>
       <c r="W7" s="7">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="X7" s="2">
         <v>0</v>
@@ -1534,7 +1558,7 @@
         <v>0</v>
       </c>
       <c r="AC7" s="21">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="AD7" s="21">
         <v>1</v>
@@ -1607,7 +1631,7 @@
       </c>
       <c r="V8" s="8"/>
       <c r="W8" s="20">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="X8" s="3">
         <v>0</v>
@@ -1625,7 +1649,7 @@
         <v>0</v>
       </c>
       <c r="AC8" s="21">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="AD8" s="8">
         <v>1</v>
@@ -1698,7 +1722,7 @@
       </c>
       <c r="V9" s="8"/>
       <c r="W9" s="7">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="X9" s="2">
         <v>0</v>
@@ -1716,7 +1740,7 @@
         <v>0</v>
       </c>
       <c r="AC9" s="21">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="AD9" s="8">
         <v>1</v>
@@ -1757,37 +1781,97 @@
       <c r="AE10" s="8"/>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.4">
-      <c r="A11" s="2"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="8"/>
-      <c r="O11" s="7"/>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="8"/>
-      <c r="R11" s="7"/>
-      <c r="S11" s="2"/>
-      <c r="T11" s="8"/>
-      <c r="U11" s="7"/>
+      <c r="A11" s="2">
+        <v>100</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="7">
+        <v>6</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="7">
+        <v>0</v>
+      </c>
+      <c r="F11" s="2">
+        <v>7</v>
+      </c>
+      <c r="G11" s="8">
+        <v>0</v>
+      </c>
+      <c r="H11" s="7">
+        <v>0</v>
+      </c>
+      <c r="I11" s="2">
+        <v>1</v>
+      </c>
+      <c r="J11" s="2">
+        <v>0</v>
+      </c>
+      <c r="K11" s="8">
+        <v>0</v>
+      </c>
+      <c r="L11" s="7">
+        <v>1</v>
+      </c>
+      <c r="M11" s="2">
+        <v>0</v>
+      </c>
+      <c r="N11" s="8">
+        <v>0</v>
+      </c>
+      <c r="O11" s="7">
+        <v>0</v>
+      </c>
+      <c r="P11" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="8">
+        <v>0</v>
+      </c>
+      <c r="R11" s="7">
+        <v>0</v>
+      </c>
+      <c r="S11" s="2">
+        <v>0</v>
+      </c>
+      <c r="T11" s="8">
+        <v>1</v>
+      </c>
+      <c r="U11" s="7">
+        <v>200</v>
+      </c>
       <c r="V11" s="8"/>
-      <c r="W11" s="7"/>
-      <c r="X11" s="2"/>
-      <c r="Y11" s="8"/>
-      <c r="Z11" s="7"/>
-      <c r="AA11" s="2"/>
-      <c r="AB11" s="2"/>
-      <c r="AC11" s="8"/>
-      <c r="AD11" s="8"/>
-      <c r="AE11" s="8"/>
+      <c r="W11" s="7">
+        <v>0</v>
+      </c>
+      <c r="X11" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="8">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="7">
+        <v>1</v>
+      </c>
+      <c r="AA11" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC11" s="8">
+        <v>0</v>
+      </c>
+      <c r="AD11" s="8">
+        <v>1</v>
+      </c>
+      <c r="AE11" s="8" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A12" s="2"/>
@@ -1823,37 +1907,97 @@
       <c r="AE12" s="8"/>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.4">
-      <c r="A13" s="2"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="8"/>
-      <c r="O13" s="7"/>
-      <c r="P13" s="2"/>
-      <c r="Q13" s="8"/>
-      <c r="R13" s="7"/>
-      <c r="S13" s="2"/>
-      <c r="T13" s="8"/>
-      <c r="U13" s="7"/>
+      <c r="A13" s="2">
+        <v>200</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="7">
+        <v>0</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="7">
+        <v>3</v>
+      </c>
+      <c r="F13" s="2">
+        <v>3</v>
+      </c>
+      <c r="G13" s="8">
+        <v>3</v>
+      </c>
+      <c r="H13" s="7">
+        <v>0</v>
+      </c>
+      <c r="I13" s="2">
+        <v>1</v>
+      </c>
+      <c r="J13" s="2">
+        <v>0</v>
+      </c>
+      <c r="K13" s="8">
+        <v>0</v>
+      </c>
+      <c r="L13" s="7">
+        <v>1</v>
+      </c>
+      <c r="M13" s="2">
+        <v>0</v>
+      </c>
+      <c r="N13" s="8">
+        <v>0</v>
+      </c>
+      <c r="O13" s="7">
+        <v>0</v>
+      </c>
+      <c r="P13" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="8">
+        <v>0</v>
+      </c>
+      <c r="R13" s="7">
+        <v>0</v>
+      </c>
+      <c r="S13" s="2">
+        <v>0</v>
+      </c>
+      <c r="T13" s="8">
+        <v>1</v>
+      </c>
+      <c r="U13" s="7">
+        <v>200</v>
+      </c>
       <c r="V13" s="8"/>
-      <c r="W13" s="7"/>
-      <c r="X13" s="2"/>
-      <c r="Y13" s="8"/>
-      <c r="Z13" s="7"/>
-      <c r="AA13" s="2"/>
-      <c r="AB13" s="2"/>
-      <c r="AC13" s="8"/>
-      <c r="AD13" s="8"/>
-      <c r="AE13" s="8"/>
+      <c r="W13" s="7">
+        <v>0</v>
+      </c>
+      <c r="X13" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="8">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="7">
+        <v>1</v>
+      </c>
+      <c r="AA13" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB13" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC13" s="8">
+        <v>0</v>
+      </c>
+      <c r="AD13" s="8">
+        <v>1</v>
+      </c>
+      <c r="AE13" s="8" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A14" s="2"/>

</xml_diff>